<commit_message>
modifications to model run
</commit_message>
<xml_diff>
--- a/inst/extdata/LandCoverCharacteristics_Soils.xlsx
+++ b/inst/extdata/LandCoverCharacteristics_Soils.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PackageDev\desertHydro\inst\extdata\DemoElements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PackageDev\desertHydro\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E4F52D-283D-44CF-8188-3300A496BB68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6D0AB6-64D6-4D1D-A179-6A273AA56FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units_m_day" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>MUSYM</t>
+  </si>
+  <si>
+    <t>infiltration_cmhr</t>
   </si>
 </sst>
 </file>
@@ -485,11 +488,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E18" sqref="E18"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,10 +515,10 @@
     <col min="19" max="19" width="36" customWidth="1"/>
     <col min="20" max="20" width="36.140625" customWidth="1"/>
     <col min="21" max="21" width="15.28515625" customWidth="1"/>
-    <col min="22" max="22" width="12" customWidth="1"/>
+    <col min="22" max="22" width="5.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -582,8 +585,11 @@
       <c r="V1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="W1" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -654,8 +660,11 @@
       <c r="V2">
         <v>0.05</v>
       </c>
+      <c r="W2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -726,8 +735,11 @@
       <c r="V3">
         <v>0.05</v>
       </c>
+      <c r="W3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -798,8 +810,11 @@
       <c r="V4">
         <v>0.05</v>
       </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -870,8 +885,11 @@
       <c r="V5">
         <v>0.05</v>
       </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -942,8 +960,11 @@
       <c r="V6">
         <v>0.05</v>
       </c>
+      <c r="W6">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1014,8 +1035,11 @@
       <c r="V7">
         <v>0.05</v>
       </c>
+      <c r="W7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1086,8 +1110,11 @@
       <c r="V8">
         <v>0.05</v>
       </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1158,8 +1185,11 @@
       <c r="V9">
         <v>0.05</v>
       </c>
+      <c r="W9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1230,8 +1260,11 @@
       <c r="V10">
         <v>0.05</v>
       </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1301,6 +1334,9 @@
       </c>
       <c r="V11">
         <v>0.05</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix bug for goes rainfall
Update default soil characteristics
</commit_message>
<xml_diff>
--- a/inst/extdata/LandCoverCharacteristics_Soils.xlsx
+++ b/inst/extdata/LandCoverCharacteristics_Soils.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PackageDev\desertHydro\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thesis\desertHydro\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6D0AB6-64D6-4D1D-A179-6A273AA56FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DC1119-1A0C-45C9-9E3F-ECA2378B772D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units_m_day" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>infiltration_cmhr</t>
+  </si>
+  <si>
+    <t>infiltration_cm_day</t>
+  </si>
+  <si>
+    <t>Ks_cmday</t>
+  </si>
+  <si>
+    <t>Ks_mmsec</t>
   </si>
 </sst>
 </file>
@@ -488,37 +497,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:Z35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P22" sqref="P22"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="3" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="3" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="36.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
     <col min="10" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" customWidth="1"/>
-    <col min="13" max="13" width="25.140625" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.109375" customWidth="1"/>
     <col min="14" max="14" width="36" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" customWidth="1"/>
-    <col min="16" max="16" width="34.28515625" customWidth="1"/>
+    <col min="15" max="15" width="24.88671875" customWidth="1"/>
+    <col min="16" max="16" width="34.33203125" customWidth="1"/>
     <col min="17" max="18" width="46" customWidth="1"/>
     <col min="19" max="19" width="36" customWidth="1"/>
-    <col min="20" max="20" width="36.140625" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" customWidth="1"/>
-    <col min="22" max="22" width="5.42578125" customWidth="1"/>
+    <col min="20" max="20" width="36.109375" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" customWidth="1"/>
+    <col min="22" max="22" width="12.77734375" customWidth="1"/>
+    <col min="23" max="23" width="19.6640625" customWidth="1"/>
+    <col min="24" max="24" width="16.88671875" customWidth="1"/>
+    <col min="25" max="25" width="14.21875" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -588,8 +601,17 @@
       <c r="W1" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="X1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -621,8 +643,7 @@
         <v>28</v>
       </c>
       <c r="K2">
-        <f>J2*2.54</f>
-        <v>71.12</v>
+        <v>76</v>
       </c>
       <c r="L2">
         <v>3.3000000000000002E-2</v>
@@ -661,10 +682,20 @@
         <v>0.05</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <f>ROUND(Y2/24, 3)</f>
+        <v>37.5</v>
+      </c>
+      <c r="X2">
+        <v>7.85</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>900</v>
+      </c>
+      <c r="Z2">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -696,8 +727,7 @@
         <v>102</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K11" si="0">J3*2.54</f>
-        <v>259.08</v>
+        <v>200</v>
       </c>
       <c r="L3">
         <v>3.3000000000000002E-2</v>
@@ -709,15 +739,15 @@
         <v>22</v>
       </c>
       <c r="O3" s="4">
-        <f t="shared" ref="O3:O11" si="1">G3</f>
+        <f t="shared" ref="O3:O11" si="0">G3</f>
         <v>0.41699999999999998</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P11" si="2">N3</f>
+        <f t="shared" ref="P3:P11" si="1">N3</f>
         <v>22</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q11" si="3">N3</f>
+        <f t="shared" ref="Q3:Q11" si="2">N3</f>
         <v>22</v>
       </c>
       <c r="R3">
@@ -736,10 +766,20 @@
         <v>0.05</v>
       </c>
       <c r="W3">
-        <v>1</v>
+        <f t="shared" ref="W3:W11" si="3">ROUND(Y3/24, 3)</f>
+        <v>25</v>
+      </c>
+      <c r="X3">
+        <v>6.25</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>600</v>
+      </c>
+      <c r="Z3">
+        <v>48.48</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -771,8 +811,7 @@
         <v>41</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
-        <v>104.14</v>
+        <v>41</v>
       </c>
       <c r="L4">
         <v>3.3000000000000002E-2</v>
@@ -784,15 +823,15 @@
         <v>22</v>
       </c>
       <c r="O4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="P4">
         <f t="shared" si="1"/>
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="P4">
+        <v>22</v>
+      </c>
+      <c r="Q4">
         <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="R4">
@@ -811,10 +850,20 @@
         <v>0.05</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="X4">
+        <v>6.25</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>600</v>
+      </c>
+      <c r="Z4">
+        <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -846,8 +895,7 @@
         <v>20</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
-        <v>50.8</v>
+        <v>200</v>
       </c>
       <c r="L5">
         <v>5.5E-2</v>
@@ -859,15 +907,15 @@
         <v>22</v>
       </c>
       <c r="O5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="1"/>
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="P5">
+        <v>22</v>
+      </c>
+      <c r="Q5">
         <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="R5">
@@ -886,10 +934,20 @@
         <v>0.05</v>
       </c>
       <c r="W5">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="X5">
+        <v>6.25</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>300</v>
+      </c>
+      <c r="Z5">
+        <v>86.88</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -921,8 +979,7 @@
         <v>28</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>71.12</v>
+        <v>200</v>
       </c>
       <c r="L6">
         <v>2.5000000000000001E-2</v>
@@ -934,17 +991,17 @@
         <v>23</v>
       </c>
       <c r="O6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="1"/>
-        <v>0.48</v>
-      </c>
-      <c r="P6">
+        <v>23</v>
+      </c>
+      <c r="Q6">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="Q6">
-        <f t="shared" si="3"/>
-        <v>23</v>
-      </c>
       <c r="R6">
         <v>1</v>
       </c>
@@ -961,10 +1018,20 @@
         <v>0.05</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>41.667000000000002</v>
+      </c>
+      <c r="X6">
+        <v>8</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -996,8 +1063,7 @@
         <v>25</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
-        <v>63.5</v>
+        <v>200</v>
       </c>
       <c r="L7">
         <v>3.3000000000000002E-2</v>
@@ -1009,17 +1075,17 @@
         <v>6</v>
       </c>
       <c r="O7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.38</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="1"/>
-        <v>0.38</v>
-      </c>
-      <c r="P7">
+        <v>6</v>
+      </c>
+      <c r="Q7">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="Q7">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
       <c r="R7">
         <v>1</v>
       </c>
@@ -1036,10 +1102,20 @@
         <v>0.05</v>
       </c>
       <c r="W7">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="X7">
+        <v>6</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>300</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1071,8 +1147,7 @@
         <v>28</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
-        <v>71.12</v>
+        <v>200</v>
       </c>
       <c r="L8">
         <v>3.3000000000000002E-2</v>
@@ -1084,15 +1159,15 @@
         <v>22</v>
       </c>
       <c r="O8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="1"/>
-        <v>0.33</v>
-      </c>
-      <c r="P8">
+        <v>22</v>
+      </c>
+      <c r="Q8">
         <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="R8">
@@ -1111,10 +1186,20 @@
         <v>0.05</v>
       </c>
       <c r="W8">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>8.3330000000000002</v>
+      </c>
+      <c r="X8">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>200</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1146,8 +1231,7 @@
         <v>23</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
-        <v>58.42</v>
+        <v>200</v>
       </c>
       <c r="L9">
         <v>3.3000000000000002E-2</v>
@@ -1159,15 +1243,15 @@
         <v>22</v>
       </c>
       <c r="O9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="1"/>
-        <v>0.41699999999999998</v>
-      </c>
-      <c r="P9">
+        <v>22</v>
+      </c>
+      <c r="Q9">
         <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="R9">
@@ -1186,10 +1270,20 @@
         <v>0.05</v>
       </c>
       <c r="W9">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="X9">
+        <v>6.25</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>600</v>
+      </c>
+      <c r="Z9">
+        <v>48.48</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1221,8 +1315,7 @@
         <v>20</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
-        <v>50.8</v>
+        <v>20</v>
       </c>
       <c r="L10">
         <v>9.5000000000000001E-2</v>
@@ -1234,17 +1327,17 @@
         <v>6</v>
       </c>
       <c r="O10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.32</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="1"/>
-        <v>0.32</v>
-      </c>
-      <c r="P10">
+        <v>6</v>
+      </c>
+      <c r="Q10">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="Q10">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
       <c r="R10">
         <v>1</v>
       </c>
@@ -1261,10 +1354,20 @@
         <v>0.05</v>
       </c>
       <c r="W10">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>41.667000000000002</v>
+      </c>
+      <c r="X10">
+        <v>4</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Z10">
+        <v>8.76</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1296,8 +1399,7 @@
         <v>26</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
-        <v>66.040000000000006</v>
+        <v>25</v>
       </c>
       <c r="L11">
         <v>3.3000000000000002E-2</v>
@@ -1309,17 +1411,17 @@
         <v>7</v>
       </c>
       <c r="O11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="1"/>
-        <v>0.40100000000000002</v>
-      </c>
-      <c r="P11">
+        <v>7</v>
+      </c>
+      <c r="Q11">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="Q11">
-        <f t="shared" si="3"/>
-        <v>7</v>
-      </c>
       <c r="R11">
         <v>1</v>
       </c>
@@ -1336,11 +1438,21 @@
         <v>0.05</v>
       </c>
       <c r="W11">
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>12.5</v>
+      </c>
+      <c r="X11">
+        <v>7</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>300</v>
+      </c>
+      <c r="Z11">
+        <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
fix the selection error
</commit_message>
<xml_diff>
--- a/inst/extdata/LandCoverCharacteristics_Soils.xlsx
+++ b/inst/extdata/LandCoverCharacteristics_Soils.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thesis\desertHydro\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DC1119-1A0C-45C9-9E3F-ECA2378B772D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D959DDB9-DD99-47DC-8C98-7D335AA46CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>Ks_mmsec</t>
+  </si>
+  <si>
+    <t>swc_wilting</t>
   </si>
 </sst>
 </file>
@@ -497,11 +500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z35"/>
+  <dimension ref="A1:AA35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z9" sqref="Z9"/>
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -529,9 +532,10 @@
     <col min="24" max="24" width="16.88671875" customWidth="1"/>
     <col min="25" max="25" width="14.21875" customWidth="1"/>
     <col min="26" max="26" width="17.6640625" customWidth="1"/>
+    <col min="27" max="27" width="11.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,8 +614,11 @@
       <c r="Z1" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="AA1" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -695,7 +702,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -779,7 +786,7 @@
         <v>48.48</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -863,7 +870,7 @@
         <v>40.799999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -947,7 +954,7 @@
         <v>86.88</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1031,7 +1038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1115,7 +1122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1199,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1283,7 +1290,7 @@
         <v>48.48</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1367,7 +1374,7 @@
         <v>8.76</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Updated script - added green and ampt infiltration
</commit_message>
<xml_diff>
--- a/inst/extdata/LandCoverCharacteristics_Soils.xlsx
+++ b/inst/extdata/LandCoverCharacteristics_Soils.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thesis\desertHydro\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D959DDB9-DD99-47DC-8C98-7D335AA46CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC95C41-4442-4697-BCD9-64A3A3CEFE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -173,7 +173,46 @@
     <t>Ks_mmsec</t>
   </si>
   <si>
-    <t>swc_wilting</t>
+    <t>Ksat_in_hr</t>
+  </si>
+  <si>
+    <t>available_water_in_ft</t>
+  </si>
+  <si>
+    <t>saturation_percent</t>
+  </si>
+  <si>
+    <t>field_capacity_percent</t>
+  </si>
+  <si>
+    <t>matric_bulk_density</t>
+  </si>
+  <si>
+    <t>organic_matter</t>
+  </si>
+  <si>
+    <t>sand_wt_percent</t>
+  </si>
+  <si>
+    <t>clay_wt_percent</t>
+  </si>
+  <si>
+    <t>soil_depth_in</t>
+  </si>
+  <si>
+    <t>wilting_percent</t>
+  </si>
+  <si>
+    <t>soil_texture_in</t>
+  </si>
+  <si>
+    <t>sand</t>
+  </si>
+  <si>
+    <t>loamy sand</t>
+  </si>
+  <si>
+    <t>sandy loam</t>
   </si>
 </sst>
 </file>
@@ -500,11 +539,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA35"/>
+  <dimension ref="A1:AN35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA2" sqref="AA2"/>
+      <pane xSplit="1" topLeftCell="Y1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE8" sqref="AE8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -532,10 +571,17 @@
     <col min="24" max="24" width="16.88671875" customWidth="1"/>
     <col min="25" max="25" width="14.21875" customWidth="1"/>
     <col min="26" max="26" width="17.6640625" customWidth="1"/>
-    <col min="27" max="27" width="11.21875" customWidth="1"/>
+    <col min="27" max="27" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.6640625" customWidth="1"/>
+    <col min="29" max="29" width="24.33203125" customWidth="1"/>
+    <col min="30" max="30" width="12.77734375" customWidth="1"/>
+    <col min="31" max="31" width="12.5546875" customWidth="1"/>
+    <col min="34" max="34" width="11.33203125" customWidth="1"/>
+    <col min="36" max="36" width="14.88671875" customWidth="1"/>
+    <col min="37" max="37" width="12.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,10 +661,40 @@
         <v>44</v>
       </c>
       <c r="AA1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE1" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AF1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -701,8 +777,42 @@
       <c r="Z2">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA2">
+        <v>1.8</v>
+      </c>
+      <c r="AB2">
+        <v>5.3</v>
+      </c>
+      <c r="AC2">
+        <v>43.7</v>
+      </c>
+      <c r="AD2">
+        <v>0.43</v>
+      </c>
+      <c r="AE2">
+        <v>5.66</v>
+      </c>
+      <c r="AF2">
+        <v>93.17</v>
+      </c>
+      <c r="AG2">
+        <v>0.8</v>
+      </c>
+      <c r="AH2">
+        <v>95</v>
+      </c>
+      <c r="AI2">
+        <v>3</v>
+      </c>
+      <c r="AJ2">
+        <f>AVERAGE(8,5)</f>
+        <v>6.5</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -785,8 +895,42 @@
       <c r="Z3">
         <v>48.48</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA3">
+        <v>1.5</v>
+      </c>
+      <c r="AB3">
+        <v>5.2</v>
+      </c>
+      <c r="AC3">
+        <v>44.7</v>
+      </c>
+      <c r="AD3">
+        <v>0.45</v>
+      </c>
+      <c r="AE3">
+        <v>6.32</v>
+      </c>
+      <c r="AF3">
+        <v>91.52</v>
+      </c>
+      <c r="AG3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AH3">
+        <v>97</v>
+      </c>
+      <c r="AI3">
+        <v>2</v>
+      </c>
+      <c r="AJ3">
+        <f>AVERAGE(7,21)</f>
+        <v>14</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -869,8 +1013,42 @@
       <c r="Z4">
         <v>40.799999999999997</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA4">
+        <v>1.8</v>
+      </c>
+      <c r="AB4">
+        <v>5.4</v>
+      </c>
+      <c r="AC4">
+        <v>42.2</v>
+      </c>
+      <c r="AD4">
+        <v>0.43</v>
+      </c>
+      <c r="AE4">
+        <v>5.04</v>
+      </c>
+      <c r="AF4">
+        <v>95.6</v>
+      </c>
+      <c r="AG4">
+        <v>0.3</v>
+      </c>
+      <c r="AH4">
+        <v>94</v>
+      </c>
+      <c r="AI4">
+        <v>4</v>
+      </c>
+      <c r="AJ4">
+        <f>17</f>
+        <v>17</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -953,8 +1131,42 @@
       <c r="Z5">
         <v>86.88</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA5">
+        <v>3</v>
+      </c>
+      <c r="AB5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="AC5">
+        <v>41.7</v>
+      </c>
+      <c r="AD5">
+        <v>0.63</v>
+      </c>
+      <c r="AE5">
+        <v>3.83</v>
+      </c>
+      <c r="AF5">
+        <v>96.45</v>
+      </c>
+      <c r="AG5">
+        <v>0.6</v>
+      </c>
+      <c r="AH5">
+        <v>85</v>
+      </c>
+      <c r="AI5">
+        <v>5</v>
+      </c>
+      <c r="AJ5">
+        <f>AVERAGE(13,35)</f>
+        <v>24</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1037,8 +1249,42 @@
       <c r="Z6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA6">
+        <v>0.9</v>
+      </c>
+      <c r="AB6">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AC6">
+        <v>43.8</v>
+      </c>
+      <c r="AD6">
+        <v>0.42</v>
+      </c>
+      <c r="AE6">
+        <v>6.86</v>
+      </c>
+      <c r="AF6">
+        <v>93.05</v>
+      </c>
+      <c r="AG6">
+        <v>0.6</v>
+      </c>
+      <c r="AH6">
+        <v>96</v>
+      </c>
+      <c r="AI6">
+        <v>2</v>
+      </c>
+      <c r="AJ6">
+        <f>AVERAGE(12,11)</f>
+        <v>11.5</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1121,8 +1367,43 @@
       <c r="Z7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AB7">
+        <v>7</v>
+      </c>
+      <c r="AC7">
+        <v>42.2</v>
+      </c>
+      <c r="AD7">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AE7">
+        <v>4.51</v>
+      </c>
+      <c r="AF7">
+        <v>95.57</v>
+      </c>
+      <c r="AG7">
+        <v>0.6</v>
+      </c>
+      <c r="AH7">
+        <f>ROUND(AVERAGE(97,78),0)</f>
+        <v>88</v>
+      </c>
+      <c r="AI7">
+        <v>4</v>
+      </c>
+      <c r="AJ7">
+        <f>AVERAGE(8,32)</f>
+        <v>20</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1205,8 +1486,42 @@
       <c r="Z8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA8">
+        <v>0.6</v>
+      </c>
+      <c r="AB8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AC8">
+        <v>42.9</v>
+      </c>
+      <c r="AD8">
+        <v>0.45</v>
+      </c>
+      <c r="AE8">
+        <v>7.22</v>
+      </c>
+      <c r="AF8">
+        <v>94.49</v>
+      </c>
+      <c r="AG8">
+        <v>0.3</v>
+      </c>
+      <c r="AH8">
+        <v>94</v>
+      </c>
+      <c r="AI8">
+        <v>2</v>
+      </c>
+      <c r="AJ8">
+        <f>AVERAGE(11)</f>
+        <v>11</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1289,8 +1604,42 @@
       <c r="Z9">
         <v>48.48</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA9">
+        <v>0.5</v>
+      </c>
+      <c r="AB9">
+        <v>4</v>
+      </c>
+      <c r="AC9">
+        <v>43.1</v>
+      </c>
+      <c r="AD9">
+        <v>0.41</v>
+      </c>
+      <c r="AE9">
+        <v>7.51</v>
+      </c>
+      <c r="AF9">
+        <v>94.05</v>
+      </c>
+      <c r="AG9">
+        <v>0.3</v>
+      </c>
+      <c r="AH9">
+        <v>96</v>
+      </c>
+      <c r="AI9">
+        <v>3</v>
+      </c>
+      <c r="AJ9">
+        <f>AVERAGE(13,9)</f>
+        <v>11</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1373,8 +1722,42 @@
       <c r="Z10">
         <v>8.76</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="AA10">
+        <v>12.1</v>
+      </c>
+      <c r="AB10">
+        <v>21.5</v>
+      </c>
+      <c r="AC10">
+        <v>39.200000000000003</v>
+      </c>
+      <c r="AD10">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="AE10">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="AF10">
+        <v>100.54</v>
+      </c>
+      <c r="AG10">
+        <v>0.3</v>
+      </c>
+      <c r="AH10">
+        <v>60</v>
+      </c>
+      <c r="AI10">
+        <v>20</v>
+      </c>
+      <c r="AJ10">
+        <f>AVERAGE(8)</f>
+        <v>8</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1457,8 +1840,84 @@
       <c r="Z11">
         <v>40.799999999999997</v>
       </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="AA11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AB11">
+        <v>11.1</v>
+      </c>
+      <c r="AC11">
+        <v>39.9</v>
+      </c>
+      <c r="AD11">
+        <v>0.77</v>
+      </c>
+      <c r="AE11">
+        <v>2.41</v>
+      </c>
+      <c r="AF11">
+        <v>99.47</v>
+      </c>
+      <c r="AG11">
+        <v>0.3</v>
+      </c>
+      <c r="AH11">
+        <v>77</v>
+      </c>
+      <c r="AI11">
+        <v>8</v>
+      </c>
+      <c r="AJ11">
+        <f>AVERAGE(6)</f>
+        <v>6</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AE15" s="1"/>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AE16" s="1"/>
+    </row>
+    <row r="17" spans="31:31" x14ac:dyDescent="0.3">
+      <c r="AE17" s="1"/>
+    </row>
+    <row r="18" spans="31:31" x14ac:dyDescent="0.3">
+      <c r="AE18" s="1"/>
+    </row>
+    <row r="19" spans="31:31" x14ac:dyDescent="0.3">
+      <c r="AE19" s="1"/>
+    </row>
+    <row r="20" spans="31:31" x14ac:dyDescent="0.3">
+      <c r="AE20" s="1"/>
+    </row>
+    <row r="21" spans="31:31" x14ac:dyDescent="0.3">
+      <c r="AE21" s="1"/>
+    </row>
+    <row r="22" spans="31:31" x14ac:dyDescent="0.3">
+      <c r="AE22" s="1"/>
+    </row>
+    <row r="23" spans="31:31" x14ac:dyDescent="0.3">
+      <c r="AE23" s="1"/>
+    </row>
+    <row r="24" spans="31:31" x14ac:dyDescent="0.3">
+      <c r="AE24" s="1"/>
+    </row>
+    <row r="26" spans="31:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reduce mannings n and increase slope. Go faster to stop the piling effect
</commit_message>
<xml_diff>
--- a/inst/extdata/LandCoverCharacteristics_Soils.xlsx
+++ b/inst/extdata/LandCoverCharacteristics_Soils.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PackageDev\desertHydro\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thesis\desertHydro\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE9AF5F-C1A8-4023-9A77-B71996CB02FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9689B80-4E44-4323-8A31-8FC75128E59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units_m_day" sheetId="1" r:id="rId1"/>
@@ -542,46 +542,46 @@
   <dimension ref="A1:AN35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="V17" sqref="V17"/>
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="3" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="3" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" style="4" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="36.88671875" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
     <col min="10" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" customWidth="1"/>
-    <col min="13" max="13" width="25.140625" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" customWidth="1"/>
+    <col min="13" max="13" width="25.109375" customWidth="1"/>
     <col min="14" max="14" width="36" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" customWidth="1"/>
-    <col min="16" max="16" width="34.28515625" customWidth="1"/>
+    <col min="15" max="15" width="24.88671875" customWidth="1"/>
+    <col min="16" max="16" width="34.33203125" customWidth="1"/>
     <col min="17" max="18" width="46" customWidth="1"/>
     <col min="19" max="19" width="36" customWidth="1"/>
-    <col min="20" max="20" width="36.140625" customWidth="1"/>
-    <col min="21" max="21" width="15.28515625" customWidth="1"/>
-    <col min="22" max="22" width="12.7109375" customWidth="1"/>
-    <col min="23" max="23" width="19.7109375" customWidth="1"/>
-    <col min="24" max="24" width="16.85546875" customWidth="1"/>
-    <col min="25" max="25" width="14.28515625" customWidth="1"/>
-    <col min="26" max="26" width="17.7109375" customWidth="1"/>
-    <col min="27" max="27" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.7109375" customWidth="1"/>
-    <col min="29" max="29" width="24.28515625" customWidth="1"/>
-    <col min="30" max="30" width="12.7109375" customWidth="1"/>
-    <col min="31" max="31" width="12.5703125" customWidth="1"/>
-    <col min="34" max="34" width="11.28515625" customWidth="1"/>
-    <col min="36" max="36" width="14.85546875" customWidth="1"/>
-    <col min="37" max="37" width="12.7109375" customWidth="1"/>
+    <col min="20" max="20" width="36.109375" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" customWidth="1"/>
+    <col min="23" max="23" width="19.6640625" customWidth="1"/>
+    <col min="24" max="24" width="16.88671875" customWidth="1"/>
+    <col min="25" max="25" width="14.33203125" customWidth="1"/>
+    <col min="26" max="26" width="17.6640625" customWidth="1"/>
+    <col min="27" max="27" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.6640625" customWidth="1"/>
+    <col min="29" max="29" width="24.33203125" customWidth="1"/>
+    <col min="30" max="30" width="12.6640625" customWidth="1"/>
+    <col min="31" max="31" width="12.5546875" customWidth="1"/>
+    <col min="34" max="34" width="11.33203125" customWidth="1"/>
+    <col min="36" max="36" width="14.88671875" customWidth="1"/>
+    <col min="37" max="37" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +694,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -762,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="V2">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="W2">
         <f>ROUND(Y2/24, 3)</f>
@@ -812,7 +812,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -880,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="V3">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="W3">
         <f t="shared" ref="W3:W11" si="3">ROUND(Y3/24, 3)</f>
@@ -930,7 +930,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -998,7 +998,7 @@
         <v>0</v>
       </c>
       <c r="V4">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="W4">
         <f t="shared" si="3"/>
@@ -1048,7 +1048,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>0</v>
       </c>
       <c r="V5">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="W5">
         <f t="shared" si="3"/>
@@ -1166,7 +1166,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="V6">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="W6">
         <f t="shared" si="3"/>
@@ -1284,7 +1284,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>35</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="W7">
         <f t="shared" si="3"/>
@@ -1403,7 +1403,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>0</v>
       </c>
       <c r="V8">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="W8">
         <f t="shared" si="3"/>
@@ -1521,7 +1521,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>0</v>
       </c>
       <c r="V9">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="W9">
         <f t="shared" si="3"/>
@@ -1639,7 +1639,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>36</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>0</v>
       </c>
       <c r="V10">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="W10">
         <f t="shared" si="3"/>
@@ -1757,7 +1757,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="V11">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="W11">
         <f t="shared" si="3"/>
@@ -1875,7 +1875,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AE14" s="1"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
@@ -1887,38 +1887,38 @@
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AE15" s="1"/>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AE16" s="1"/>
     </row>
-    <row r="17" spans="31:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="31:31" x14ac:dyDescent="0.3">
       <c r="AE17" s="1"/>
     </row>
-    <row r="18" spans="31:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="31:31" x14ac:dyDescent="0.3">
       <c r="AE18" s="1"/>
     </row>
-    <row r="19" spans="31:31" x14ac:dyDescent="0.25">
+    <row r="19" spans="31:31" x14ac:dyDescent="0.3">
       <c r="AE19" s="1"/>
     </row>
-    <row r="20" spans="31:31" x14ac:dyDescent="0.25">
+    <row r="20" spans="31:31" x14ac:dyDescent="0.3">
       <c r="AE20" s="1"/>
     </row>
-    <row r="21" spans="31:31" x14ac:dyDescent="0.25">
+    <row r="21" spans="31:31" x14ac:dyDescent="0.3">
       <c r="AE21" s="1"/>
     </row>
-    <row r="22" spans="31:31" x14ac:dyDescent="0.25">
+    <row r="22" spans="31:31" x14ac:dyDescent="0.3">
       <c r="AE22" s="1"/>
     </row>
-    <row r="23" spans="31:31" x14ac:dyDescent="0.25">
+    <row r="23" spans="31:31" x14ac:dyDescent="0.3">
       <c r="AE23" s="1"/>
     </row>
-    <row r="24" spans="31:31" x14ac:dyDescent="0.25">
+    <row r="24" spans="31:31" x14ac:dyDescent="0.3">
       <c r="AE24" s="1"/>
     </row>
-    <row r="26" spans="31:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="31:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="13.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>